<commit_message>
Colromap and title also for dS
</commit_message>
<xml_diff>
--- a/CVX_Kenya/Optimization/ Pulping_machines_450_109.xlsx
+++ b/CVX_Kenya/Optimization/ Pulping_machines_450_109.xlsx
@@ -555,37 +555,37 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>400.9907172536477</v>
+        <v>1.00000015925616</v>
       </c>
       <c r="G4">
-        <v>-0.9994304059073329</v>
+        <v>0.6107773305848241</v>
       </c>
       <c r="H4">
-        <v>-401.219249367952</v>
+        <v>1.63725814495874</v>
       </c>
       <c r="I4">
-        <v>-0.05114082011277787</v>
+        <v>0.002327894559130073</v>
       </c>
       <c r="J4">
-        <v>-0.01008209880092181</v>
+        <v>0.002149965708667878</v>
       </c>
       <c r="K4">
-        <v>-0.2510589539306238</v>
+        <v>0.3085486581549048</v>
       </c>
       <c r="L4">
-        <v>-0.1366259895730764</v>
+        <v>0.03071292489767075</v>
       </c>
       <c r="M4">
-        <v>1.799733230887796</v>
+        <v>0.0006180771888466552</v>
       </c>
       <c r="N4">
-        <v>1.096701021939225</v>
+        <v>0.2859652930637822</v>
       </c>
       <c r="O4">
-        <v>0.4893780273851007</v>
+        <v>0.0001950151054188609</v>
       </c>
       <c r="P4">
-        <v>20.56325181527063</v>
+        <v>0.09720575390383601</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor changes in charts of single interventions
- Try to plot always only what is useful to explaining the specific intervention
- Always plot in K USD since we decide to use this for easier comparability
</commit_message>
<xml_diff>
--- a/CVX_Kenya/Optimization/ Pulping_machines_450_109.xlsx
+++ b/CVX_Kenya/Optimization/ Pulping_machines_450_109.xlsx
@@ -555,37 +555,37 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>5421.299537870102</v>
+        <v>1.00000015925616</v>
       </c>
       <c r="G4">
-        <v>3253.734504770488</v>
+        <v>0.6107773305848241</v>
       </c>
       <c r="H4">
-        <v>1.666177596826546</v>
+        <v>1.63725814495874</v>
       </c>
       <c r="I4">
-        <v>9.686076806276105</v>
+        <v>0.002327894559130073</v>
       </c>
       <c r="J4">
-        <v>58.23311956987891</v>
+        <v>0.002149965708667878</v>
       </c>
       <c r="K4">
-        <v>3.371160993818194</v>
+        <v>0.3085486581549048</v>
       </c>
       <c r="L4">
-        <v>75.68173810420558</v>
+        <v>0.03071292489767075</v>
       </c>
       <c r="M4">
-        <v>24.33238917902054</v>
+        <v>0.0006180771888466552</v>
       </c>
       <c r="N4">
-        <v>14.82826949442824</v>
+        <v>0.2859652930637822</v>
       </c>
       <c r="O4">
-        <v>6.616823517833836</v>
+        <v>0.0001950151054188609</v>
       </c>
       <c r="P4">
-        <v>278.0264926441014</v>
+        <v>0.09720575390383601</v>
       </c>
     </row>
   </sheetData>

</xml_diff>